<commit_message>
balas, mueren enemigos y lista actualizada
</commit_message>
<xml_diff>
--- a/Documentos/Lista_entregables.xlsx
+++ b/Documentos/Lista_entregables.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nereacastellanosrodriguez/Desktop/Universidad/CUARTO - ABP/github/Vesper/Documentos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Stoycho/GitHub/Vesper/Documentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,9 +16,6 @@
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -1452,8 +1449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="B102" sqref="B102"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="F120" sqref="F120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2741,12 +2738,12 @@
       <c r="C117" s="64"/>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A118" s="56" t="s">
+      <c r="A118" s="75" t="s">
         <v>132</v>
       </c>
-      <c r="B118" s="56"/>
-      <c r="C118" s="57"/>
-      <c r="D118" t="s">
+      <c r="B118" s="75"/>
+      <c r="C118" s="76"/>
+      <c r="D118" s="77" t="s">
         <v>145</v>
       </c>
     </row>
@@ -2757,7 +2754,7 @@
       <c r="B119" s="63"/>
       <c r="C119" s="64"/>
     </row>
-    <row r="120" spans="1:4" s="77" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:4" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A120" s="75" t="s">
         <v>134</v>
       </c>
@@ -2788,7 +2785,7 @@
       <c r="B123" s="65"/>
       <c r="C123" s="65"/>
     </row>
-    <row r="124" spans="1:4" s="77" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:4" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A124" s="75" t="s">
         <v>138</v>
       </c>
@@ -2798,7 +2795,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="125" spans="1:4" s="77" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:4" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A125" s="75" t="s">
         <v>139</v>
       </c>
@@ -2819,12 +2816,12 @@
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A127" s="56" t="s">
+      <c r="A127" s="75" t="s">
         <v>141</v>
       </c>
-      <c r="B127" s="58"/>
-      <c r="C127" s="58"/>
-      <c r="D127" t="s">
+      <c r="B127" s="78"/>
+      <c r="C127" s="78"/>
+      <c r="D127" s="77" t="s">
         <v>142</v>
       </c>
     </row>

</xml_diff>

<commit_message>
lista de entregarles actualizada
</commit_message>
<xml_diff>
--- a/Documentos/Lista_entregables.xlsx
+++ b/Documentos/Lista_entregables.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gasparrodriguezvalero/GitHub/Vesper/Documentos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Catherine/Documents/GitHub/Vesper/Documentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="177">
   <si>
     <t>HITO 1</t>
   </si>
@@ -522,6 +522,42 @@
   </si>
   <si>
     <t xml:space="preserve">Bounding Box </t>
+  </si>
+  <si>
+    <t>Diseño de los mapas (Colocar los objetos en Tiled)</t>
+  </si>
+  <si>
+    <t>Arreglar puerta y llave en release</t>
+  </si>
+  <si>
+    <t>Disparos distintos según arma</t>
+  </si>
+  <si>
+    <t>Menús en general (nivel en la pantalla seleccionar y meter pantallas finales, créditos)</t>
+  </si>
+  <si>
+    <t>HUD (Llaves + mini mapa)</t>
+  </si>
+  <si>
+    <t>Balas</t>
+  </si>
+  <si>
+    <t>Modelado</t>
+  </si>
+  <si>
+    <t>Texturizado</t>
+  </si>
+  <si>
+    <t>Animaciones</t>
+  </si>
+  <si>
+    <t>Sombras</t>
+  </si>
+  <si>
+    <t>Shadder Cartoon</t>
+  </si>
+  <si>
+    <t>Sonido/Música</t>
   </si>
 </sst>
 </file>
@@ -934,7 +970,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1127,6 +1163,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1771,10 +1812,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I183"/>
+  <dimension ref="A1:I195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A135" zoomScale="125" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="A140" sqref="A140"/>
+    <sheetView tabSelected="1" topLeftCell="A171" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="A196" sqref="A196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4006,54 +4047,127 @@
         <v>154</v>
       </c>
     </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A175" s="130"/>
+      <c r="B175" s="49"/>
+      <c r="C175" s="128"/>
+      <c r="D175" s="129"/>
+      <c r="E175" s="128"/>
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B176" s="119" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A177" s="120" t="s">
+        <v>151</v>
+      </c>
+      <c r="B177">
+        <f>SUMIF($F$131:$F$174,A177,$E$131:$E$174)</f>
+        <v>198</v>
+      </c>
+    </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B178" s="119" t="s">
-        <v>156</v>
+      <c r="A178" s="120" t="s">
+        <v>152</v>
+      </c>
+      <c r="B178">
+        <f>SUMIF($F$131:$F$174,A178,$E$131:$E$174)</f>
+        <v>370</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A179" s="120" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B179">
         <f>SUMIF($F$131:$F$174,A179,$E$131:$E$174)</f>
-        <v>198</v>
+        <v>132.5</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A180" s="120" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B180">
         <f>SUMIF($F$131:$F$174,A180,$E$131:$E$174)</f>
-        <v>370</v>
+        <v>170</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A181" s="120" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B181">
         <f>SUMIF($F$131:$F$174,A181,$E$131:$E$174)</f>
-        <v>132.5</v>
+        <v>140</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A182" s="120" t="s">
-        <v>154</v>
-      </c>
-      <c r="B182">
-        <f>SUMIF($F$131:$F$174,A182,$E$131:$E$174)</f>
+      <c r="A182" s="120"/>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A183" s="120"/>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A183" s="120" t="s">
-        <v>155</v>
-      </c>
-      <c r="B183">
-        <f>SUMIF($F$131:$F$174,A183,$E$131:$E$174)</f>
-        <v>140</v>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A192" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A193" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A194" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A195" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -4147,7 +4261,7 @@
       <formula>(#REF!=2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A173:A174">
+  <conditionalFormatting sqref="A173:A175">
     <cfRule type="expression" dxfId="2" priority="2">
       <formula>(#REF!=2)</formula>
     </cfRule>

</xml_diff>